<commit_message>
Changed output file to csv, added function to detect captcha and wait for it to be solved
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -566,87 +566,87 @@
       </c>
       <c r="AA1" s="1" t="inlineStr">
         <is>
-          <t>Product15</t>
+          <t>Unnamed: 26</t>
         </is>
       </c>
       <c r="AB1" s="1" t="inlineStr">
         <is>
-          <t>Product16</t>
+          <t>Unnamed: 27</t>
         </is>
       </c>
       <c r="AC1" s="1" t="inlineStr">
         <is>
-          <t>Product17</t>
+          <t>Unnamed: 28</t>
         </is>
       </c>
       <c r="AD1" s="1" t="inlineStr">
         <is>
-          <t>Product18</t>
+          <t>Unnamed: 29</t>
         </is>
       </c>
       <c r="AE1" s="1" t="inlineStr">
         <is>
-          <t>Product19</t>
+          <t>Unnamed: 30</t>
         </is>
       </c>
       <c r="AF1" s="1" t="inlineStr">
         <is>
-          <t>Product20</t>
+          <t>Unnamed: 31</t>
         </is>
       </c>
       <c r="AG1" s="1" t="inlineStr">
         <is>
-          <t>Product21</t>
+          <t>Unnamed: 32</t>
         </is>
       </c>
       <c r="AH1" s="1" t="inlineStr">
         <is>
-          <t>Product22</t>
+          <t>Unnamed: 33</t>
         </is>
       </c>
       <c r="AI1" s="1" t="inlineStr">
         <is>
-          <t>Product23</t>
+          <t>Unnamed: 34</t>
         </is>
       </c>
       <c r="AJ1" s="1" t="inlineStr">
         <is>
-          <t>Product24</t>
+          <t>Unnamed: 35</t>
         </is>
       </c>
       <c r="AK1" s="1" t="inlineStr">
         <is>
-          <t>Product25</t>
+          <t>Unnamed: 36</t>
         </is>
       </c>
       <c r="AL1" s="1" t="inlineStr">
         <is>
-          <t>Product26</t>
+          <t>Unnamed: 37</t>
         </is>
       </c>
       <c r="AM1" s="1" t="inlineStr">
         <is>
-          <t>Product27</t>
+          <t>Unnamed: 38</t>
         </is>
       </c>
       <c r="AN1" s="1" t="inlineStr">
         <is>
-          <t>Product28</t>
+          <t>Unnamed: 39</t>
         </is>
       </c>
       <c r="AO1" s="1" t="inlineStr">
         <is>
-          <t>Product29</t>
+          <t>Unnamed: 40</t>
         </is>
       </c>
       <c r="AP1" s="1" t="inlineStr">
         <is>
-          <t>Product30</t>
+          <t>Unnamed: 41</t>
         </is>
       </c>
       <c r="AQ1" s="1" t="inlineStr">
         <is>
-          <t>Product31</t>
+          <t>Unnamed: 42</t>
         </is>
       </c>
       <c r="AR1" s="1" t="inlineStr">
@@ -1951,7 +1951,7 @@
       </c>
       <c r="AA6" t="inlineStr">
         <is>
-          <t>Wire &amp; Cable</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="AB6" t="inlineStr">
@@ -2630,24 +2630,12 @@
       </c>
       <c r="AZ8" t="inlineStr">
         <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="BA8" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="BB8" t="inlineStr">
-        <is>
-          <t>https://www.google.com/search?q=inurl%3Astockwell.com+%28%22quick+change+connector%22+OR+%22connector%22+OR+%22quick+disconnect+connector%22+OR+%22quick+connector%22+OR+%22fluid+connector%22+OR+%22hydraulic+connector%22+or+%22hydraulic%22+or+%22fluid%22%29+%28product+OR+buy+OR+shop+OR+store+OR+price+OR+catalog+OR+%0A++++++++++++specifications%29</t>
-        </is>
-      </c>
-      <c r="BC8" t="inlineStr">
-        <is>
-          <t>https://www.google.com/search?q=inurl%3Astockwell.com+%28%22quick+change+connector%22+OR+%22connector%22+OR+%22quick+disconnect+connector%22+OR+%22quick+connector%22+OR+%22fluid+connector%22+OR+%22hydraulic+connector%22+or+%22hydraulic%22+or+%22fluid%22%29+%28product+OR+buy+OR+shop+OR+store+OR+price+OR+catalog+OR+%0A++++++++++++specifications%29</t>
-        </is>
-      </c>
+          <t>https://www.stockwell.com/technical-tips/</t>
+        </is>
+      </c>
+      <c r="BA8" t="inlineStr"/>
+      <c r="BB8" t="inlineStr"/>
+      <c r="BC8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -3336,87 +3324,87 @@
       </c>
       <c r="AA11" t="inlineStr">
         <is>
-          <t>Density</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="AB11" t="inlineStr">
         <is>
-          <t>Meter Provers</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="AC11" t="inlineStr">
         <is>
-          <t>Regulators</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="AD11" t="inlineStr">
         <is>
-          <t>Sensors</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="AE11" t="inlineStr">
         <is>
-          <t>Temperature</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="AF11" t="inlineStr">
         <is>
-          <t>Instrument Accessories</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="AG11" t="inlineStr">
         <is>
-          <t>Terminal Blocks</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="AH11" t="inlineStr">
         <is>
-          <t>HMI/SCADA</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="AI11" t="inlineStr">
         <is>
-          <t>Signal Devices</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="AJ11" t="inlineStr">
         <is>
-          <t>Variable Speed Drives</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="AK11" t="inlineStr">
         <is>
-          <t>Relays</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="AL11" t="inlineStr">
         <is>
-          <t>Fuses</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="AM11" t="inlineStr">
         <is>
-          <t>Industrial Networks</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="AN11" t="inlineStr">
         <is>
-          <t>Control Accessories</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="AO11" t="inlineStr">
         <is>
-          <t>Fire Alarm Devices</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="AP11" t="inlineStr">
         <is>
-          <t>Gas Detectors</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="AQ11" t="inlineStr">
         <is>
-          <t>Calibration Gas</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="AR11" t="inlineStr">
@@ -3461,24 +3449,12 @@
       </c>
       <c r="AZ11" t="inlineStr">
         <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="BA11" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="BB11" t="inlineStr">
-        <is>
-          <t>https://www.google.com/search?q=inurl%3Agilautomation.com+%28%22quick+change+connector%22+OR+%22connector%22+OR+%22quick+disconnect+connector%22+OR+%22quick+connector%22+OR+%22fluid+connector%22+OR+%22hydraulic+connector%22+or+%22hydraulic%22+or+%22fluid%22%29+%28product+OR+buy+OR+shop+OR+store+OR+price+OR+catalog+OR+%0A++++++++++++specifications%29</t>
-        </is>
-      </c>
-      <c r="BC11" t="inlineStr">
-        <is>
-          <t>https://www.google.com/search?q=inurl%3Agilautomation.com+%28%22quick+change+connector%22+OR+%22connector%22+OR+%22quick+disconnect+connector%22+OR+%22quick+connector%22+OR+%22fluid+connector%22+OR+%22hydraulic+connector%22+or+%22hydraulic%22+or+%22fluid%22%29+%28product+OR+buy+OR+shop+OR+store+OR+price+OR+catalog+OR+%0A++++++++++++specifications%29</t>
-        </is>
-      </c>
+          <t>https://www.gilautomation.com/collections/pumps</t>
+        </is>
+      </c>
+      <c r="BA11" t="inlineStr"/>
+      <c r="BB11" t="inlineStr"/>
+      <c r="BC11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -5401,24 +5377,16 @@
       </c>
       <c r="AZ18" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>https://www.triadtechnologies.com/fluid-connectors/quick-couplings.html</t>
         </is>
       </c>
       <c r="BA18" t="inlineStr">
         <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="BB18" t="inlineStr">
-        <is>
-          <t>https://www.google.com/search?q=inurl%3Atriadtechnologies.com+%28%22quick+change+connector%22+OR+%22connector%22+OR+%22quick+disconnect+connector%22+OR+%22quick+connector%22+OR+%22fluid+connector%22+OR+%22hydraulic+connector%22+or+%22hydraulic%22+or+%22fluid%22%29+%28product+OR+buy+OR+shop+OR+store+OR+price+OR+catalog+OR+%0A++++++++++++specifications%29</t>
-        </is>
-      </c>
-      <c r="BC18" t="inlineStr">
-        <is>
-          <t>https://www.google.com/search?q=inurl%3Atriadtechnologies.com+%28%22quick+change+connector%22+OR+%22connector%22+OR+%22quick+disconnect+connector%22+OR+%22quick+connector%22+OR+%22fluid+connector%22+OR+%22hydraulic+connector%22+or+%22hydraulic%22+or+%22fluid%22%29+%28product+OR+buy+OR+shop+OR+store+OR+price+OR+catalog+OR+%0A++++++++++++specifications%29</t>
-        </is>
-      </c>
+          <t>https://www.triadtechnologies.com/fluid-connectors/quick-couplings.html</t>
+        </is>
+      </c>
+      <c r="BB18" t="inlineStr"/>
+      <c r="BC18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -5953,26 +5921,10 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="AZ20" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="BA20" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="BB20" t="inlineStr">
-        <is>
-          <t>https://www.google.com/search?q=inurl%3Aeurotherm.com+%28%22quick+change+connector%22+OR+%22connector%22+OR+%22quick+disconnect+connector%22+OR+%22quick+connector%22+OR+%22fluid+connector%22+OR+%22hydraulic+connector%22+or+%22hydraulic%22+or+%22fluid%22%29+%28product+OR+buy+OR+shop+OR+store+OR+price+OR+catalog+OR+%0A++++++++++++specifications%29</t>
-        </is>
-      </c>
-      <c r="BC20" t="inlineStr">
-        <is>
-          <t>https://www.google.com/search?q=inurl%3Aeurotherm.com+%28%22quick+change+connector%22+OR+%22connector%22+OR+%22quick+disconnect+connector%22+OR+%22quick+connector%22+OR+%22fluid+connector%22+OR+%22hydraulic+connector%22+or+%22hydraulic%22+or+%22fluid%22%29+%28product+OR+buy+OR+shop+OR+store+OR+price+OR+catalog+OR+%0A++++++++++++specifications%29</t>
-        </is>
-      </c>
+      <c r="AZ20" t="inlineStr"/>
+      <c r="BA20" t="inlineStr"/>
+      <c r="BB20" t="inlineStr"/>
+      <c r="BC20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -6230,26 +6182,10 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="AZ21" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="BA21" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="BB21" t="inlineStr">
-        <is>
-          <t>https://www.google.com/search?q=inurl%3Aamphenol-industrial.com+%28%22quick+change+connector%22+OR+%22connector%22+OR+%22quick+disconnect+connector%22+OR+%22quick+connector%22+OR+%22fluid+connector%22+OR+%22hydraulic+connector%22+or+%22hydraulic%22+or+%22fluid%22%29+%28product+OR+buy+OR+shop+OR+store+OR+price+OR+catalog+OR+%0A++++++++++++specifications%29</t>
-        </is>
-      </c>
-      <c r="BC21" t="inlineStr">
-        <is>
-          <t>https://www.google.com/search?q=inurl%3Aamphenol-industrial.com+%28%22quick+change+connector%22+OR+%22connector%22+OR+%22quick+disconnect+connector%22+OR+%22quick+connector%22+OR+%22fluid+connector%22+OR+%22hydraulic+connector%22+or+%22hydraulic%22+or+%22fluid%22%29+%28product+OR+buy+OR+shop+OR+store+OR+price+OR+catalog+OR+%0A++++++++++++specifications%29</t>
-        </is>
-      </c>
+      <c r="AZ21" t="inlineStr"/>
+      <c r="BA21" t="inlineStr"/>
+      <c r="BB21" t="inlineStr"/>
+      <c r="BC21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -6507,26 +6443,10 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="AZ22" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="BA22" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="BB22" t="inlineStr">
-        <is>
-          <t>https://www.google.com/search?q=inurl%3Atherm-x.com+%28%22quick+change+connector%22+OR+%22connector%22+OR+%22quick+disconnect+connector%22+OR+%22quick+connector%22+OR+%22fluid+connector%22+OR+%22hydraulic+connector%22+or+%22hydraulic%22+or+%22fluid%22%29+%28product+OR+buy+OR+shop+OR+store+OR+price+OR+catalog+OR+%0A++++++++++++specifications%29</t>
-        </is>
-      </c>
-      <c r="BC22" t="inlineStr">
-        <is>
-          <t>https://www.google.com/search?q=inurl%3Atherm-x.com+%28%22quick+change+connector%22+OR+%22connector%22+OR+%22quick+disconnect+connector%22+OR+%22quick+connector%22+OR+%22fluid+connector%22+OR+%22hydraulic+connector%22+or+%22hydraulic%22+or+%22fluid%22%29+%28product+OR+buy+OR+shop+OR+store+OR+price+OR+catalog+OR+%0A++++++++++++specifications%29</t>
-        </is>
-      </c>
+      <c r="AZ22" t="inlineStr"/>
+      <c r="BA22" t="inlineStr"/>
+      <c r="BB22" t="inlineStr"/>
+      <c r="BC22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -6784,26 +6704,10 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="AZ23" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="BA23" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="BB23" t="inlineStr">
-        <is>
-          <t>https://www.google.com/search?q=inurl%3Anexans.us+%28%22quick+change+connector%22+OR+%22connector%22+OR+%22quick+disconnect+connector%22+OR+%22quick+connector%22+OR+%22fluid+connector%22+OR+%22hydraulic+connector%22+or+%22hydraulic%22+or+%22fluid%22%29+%28product+OR+buy+OR+shop+OR+store+OR+price+OR+catalog+OR+%0A++++++++++++specifications%29</t>
-        </is>
-      </c>
-      <c r="BC23" t="inlineStr">
-        <is>
-          <t>https://www.google.com/search?q=inurl%3Anexans.us+%28%22quick+change+connector%22+OR+%22connector%22+OR+%22quick+disconnect+connector%22+OR+%22quick+connector%22+OR+%22fluid+connector%22+OR+%22hydraulic+connector%22+or+%22hydraulic%22+or+%22fluid%22%29+%28product+OR+buy+OR+shop+OR+store+OR+price+OR+catalog+OR+%0A++++++++++++specifications%29</t>
-        </is>
-      </c>
+      <c r="AZ23" t="inlineStr"/>
+      <c r="BA23" t="inlineStr"/>
+      <c r="BB23" t="inlineStr"/>
+      <c r="BC23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -7061,26 +6965,10 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="AZ24" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="BA24" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="BB24" t="inlineStr">
-        <is>
-          <t>https://www.google.com/search?q=inurl%3Afralock.com+%28%22quick+change+connector%22+OR+%22connector%22+OR+%22quick+disconnect+connector%22+OR+%22quick+connector%22+OR+%22fluid+connector%22+OR+%22hydraulic+connector%22+or+%22hydraulic%22+or+%22fluid%22%29+%28product+OR+buy+OR+shop+OR+store+OR+price+OR+catalog+OR+%0A++++++++++++specifications%29</t>
-        </is>
-      </c>
-      <c r="BC24" t="inlineStr">
-        <is>
-          <t>https://www.google.com/search?q=inurl%3Afralock.com+%28%22quick+change+connector%22+OR+%22connector%22+OR+%22quick+disconnect+connector%22+OR+%22quick+connector%22+OR+%22fluid+connector%22+OR+%22hydraulic+connector%22+or+%22hydraulic%22+or+%22fluid%22%29+%28product+OR+buy+OR+shop+OR+store+OR+price+OR+catalog+OR+%0A++++++++++++specifications%29</t>
-        </is>
-      </c>
+      <c r="AZ24" t="inlineStr"/>
+      <c r="BA24" t="inlineStr"/>
+      <c r="BB24" t="inlineStr"/>
+      <c r="BC24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -7215,82 +7103,82 @@
       </c>
       <c r="AA25" t="inlineStr">
         <is>
-          <t>Motor Controls</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="AB25" t="inlineStr">
         <is>
-          <t>Networks</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="AC25" t="inlineStr">
         <is>
-          <t>Photoelectric Sensors</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="AD25" t="inlineStr">
         <is>
-          <t>Pilot Devices</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="AE25" t="inlineStr">
         <is>
-          <t>Power Supplies</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="AF25" t="inlineStr">
         <is>
-          <t>Pressure Sensors</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="AG25" t="inlineStr">
         <is>
-          <t>Relays and Timers</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="AH25" t="inlineStr">
         <is>
-          <t>RFID</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="AI25" t="inlineStr">
         <is>
-          <t>Safety Mats</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="AJ25" t="inlineStr">
         <is>
-          <t>Safety Modules</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="AK25" t="inlineStr">
         <is>
-          <t>Safety Switches</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="AL25" t="inlineStr">
         <is>
-          <t>Stepper Drives</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="AM25" t="inlineStr">
         <is>
-          <t>Temperature/Process Control</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="AN25" t="inlineStr">
         <is>
-          <t>Ultrasonic Sensors</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="AO25" t="inlineStr">
         <is>
-          <t>Vision Sensors/Systems</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="AP25" t="inlineStr">
         <is>
-          <t>Visual Signals</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="AQ25" t="inlineStr">
@@ -7338,26 +7226,10 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="AZ25" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="BA25" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="BB25" t="inlineStr">
-        <is>
-          <t>https://www.google.com/search?q=inurl%3Awalkerindustrial.com+%28%22quick+change+connector%22+OR+%22connector%22+OR+%22quick+disconnect+connector%22+OR+%22quick+connector%22+OR+%22fluid+connector%22+OR+%22hydraulic+connector%22+or+%22hydraulic%22+or+%22fluid%22%29+%28product+OR+buy+OR+shop+OR+store+OR+price+OR+catalog+OR+%0A++++++++++++specifications%29</t>
-        </is>
-      </c>
-      <c r="BC25" t="inlineStr">
-        <is>
-          <t>https://www.google.com/search?q=inurl%3Awalkerindustrial.com+%28%22quick+change+connector%22+OR+%22connector%22+OR+%22quick+disconnect+connector%22+OR+%22quick+connector%22+OR+%22fluid+connector%22+OR+%22hydraulic+connector%22+or+%22hydraulic%22+or+%22fluid%22%29+%28product+OR+buy+OR+shop+OR+store+OR+price+OR+catalog+OR+%0A++++++++++++specifications%29</t>
-        </is>
-      </c>
+      <c r="AZ25" t="inlineStr"/>
+      <c r="BA25" t="inlineStr"/>
+      <c r="BB25" t="inlineStr"/>
+      <c r="BC25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -7615,26 +7487,10 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="AZ26" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="BA26" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="BB26" t="inlineStr">
-        <is>
-          <t>https://www.google.com/search?q=inurl%3Awinn-marion.com+%28%22quick+change+connector%22+OR+%22connector%22+OR+%22quick+disconnect+connector%22+OR+%22quick+connector%22+OR+%22fluid+connector%22+OR+%22hydraulic+connector%22+or+%22hydraulic%22+or+%22fluid%22%29+%28product+OR+buy+OR+shop+OR+store+OR+price+OR+catalog+OR+%0A++++++++++++specifications%29</t>
-        </is>
-      </c>
-      <c r="BC26" t="inlineStr">
-        <is>
-          <t>https://www.google.com/search?q=inurl%3Awinn-marion.com+%28%22quick+change+connector%22+OR+%22connector%22+OR+%22quick+disconnect+connector%22+OR+%22quick+connector%22+OR+%22fluid+connector%22+OR+%22hydraulic+connector%22+or+%22hydraulic%22+or+%22fluid%22%29+%28product+OR+buy+OR+shop+OR+store+OR+price+OR+catalog+OR+%0A++++++++++++specifications%29</t>
-        </is>
-      </c>
+      <c r="AZ26" t="inlineStr"/>
+      <c r="BA26" t="inlineStr"/>
+      <c r="BB26" t="inlineStr"/>
+      <c r="BC26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -7892,26 +7748,10 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="AZ27" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="BA27" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="BB27" t="inlineStr">
-        <is>
-          <t>https://www.google.com/search?q=inurl%3Acypressindustries.com+%28%22quick+change+connector%22+OR+%22connector%22+OR+%22quick+disconnect+connector%22+OR+%22quick+connector%22+OR+%22fluid+connector%22+OR+%22hydraulic+connector%22+or+%22hydraulic%22+or+%22fluid%22%29+%28product+OR+buy+OR+shop+OR+store+OR+price+OR+catalog+OR+%0A++++++++++++specifications%29</t>
-        </is>
-      </c>
-      <c r="BC27" t="inlineStr">
-        <is>
-          <t>https://www.google.com/search?q=inurl%3Acypressindustries.com+%28%22quick+change+connector%22+OR+%22connector%22+OR+%22quick+disconnect+connector%22+OR+%22quick+connector%22+OR+%22fluid+connector%22+OR+%22hydraulic+connector%22+or+%22hydraulic%22+or+%22fluid%22%29+%28product+OR+buy+OR+shop+OR+store+OR+price+OR+catalog+OR+%0A++++++++++++specifications%29</t>
-        </is>
-      </c>
+      <c r="AZ27" t="inlineStr"/>
+      <c r="BA27" t="inlineStr"/>
+      <c r="BB27" t="inlineStr"/>
+      <c r="BC27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -8169,26 +8009,10 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="AZ28" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="BA28" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="BB28" t="inlineStr">
-        <is>
-          <t>https://www.google.com/search?q=inurl%3Aawcwire.com+%28%22quick+change+connector%22+OR+%22connector%22+OR+%22quick+disconnect+connector%22+OR+%22quick+connector%22+OR+%22fluid+connector%22+OR+%22hydraulic+connector%22+or+%22hydraulic%22+or+%22fluid%22%29+%28product+OR+buy+OR+shop+OR+store+OR+price+OR+catalog+OR+%0A++++++++++++specifications%29</t>
-        </is>
-      </c>
-      <c r="BC28" t="inlineStr">
-        <is>
-          <t>https://www.google.com/search?q=inurl%3Aawcwire.com+%28%22quick+change+connector%22+OR+%22connector%22+OR+%22quick+disconnect+connector%22+OR+%22quick+connector%22+OR+%22fluid+connector%22+OR+%22hydraulic+connector%22+or+%22hydraulic%22+or+%22fluid%22%29+%28product+OR+buy+OR+shop+OR+store+OR+price+OR+catalog+OR+%0A++++++++++++specifications%29</t>
-        </is>
-      </c>
+      <c r="AZ28" t="inlineStr"/>
+      <c r="BA28" t="inlineStr"/>
+      <c r="BB28" t="inlineStr"/>
+      <c r="BC28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -8446,26 +8270,10 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="AZ29" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="BA29" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="BB29" t="inlineStr">
-        <is>
-          <t>https://www.google.com/search?q=inurl%3Alexproducts.com+%28%22quick+change+connector%22+OR+%22connector%22+OR+%22quick+disconnect+connector%22+OR+%22quick+connector%22+OR+%22fluid+connector%22+OR+%22hydraulic+connector%22+or+%22hydraulic%22+or+%22fluid%22%29+%28product+OR+buy+OR+shop+OR+store+OR+price+OR+catalog+OR+%0A++++++++++++specifications%29</t>
-        </is>
-      </c>
-      <c r="BC29" t="inlineStr">
-        <is>
-          <t>https://www.google.com/search?q=inurl%3Alexproducts.com+%28%22quick+change+connector%22+OR+%22connector%22+OR+%22quick+disconnect+connector%22+OR+%22quick+connector%22+OR+%22fluid+connector%22+OR+%22hydraulic+connector%22+or+%22hydraulic%22+or+%22fluid%22%29+%28product+OR+buy+OR+shop+OR+store+OR+price+OR+catalog+OR+%0A++++++++++++specifications%29</t>
-        </is>
-      </c>
+      <c r="AZ29" t="inlineStr"/>
+      <c r="BA29" t="inlineStr"/>
+      <c r="BB29" t="inlineStr"/>
+      <c r="BC29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -8723,26 +8531,10 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="AZ30" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="BA30" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="BB30" t="inlineStr">
-        <is>
-          <t>https://www.google.com/search?q=inurl%3Aheilindasia.com+%28%22quick+change+connector%22+OR+%22connector%22+OR+%22quick+disconnect+connector%22+OR+%22quick+connector%22+OR+%22fluid+connector%22+OR+%22hydraulic+connector%22+or+%22hydraulic%22+or+%22fluid%22%29+%28product+OR+buy+OR+shop+OR+store+OR+price+OR+catalog+OR+%0A++++++++++++specifications%29</t>
-        </is>
-      </c>
-      <c r="BC30" t="inlineStr">
-        <is>
-          <t>https://www.google.com/search?q=inurl%3Aheilindasia.com+%28%22quick+change+connector%22+OR+%22connector%22+OR+%22quick+disconnect+connector%22+OR+%22quick+connector%22+OR+%22fluid+connector%22+OR+%22hydraulic+connector%22+or+%22hydraulic%22+or+%22fluid%22%29+%28product+OR+buy+OR+shop+OR+store+OR+price+OR+catalog+OR+%0A++++++++++++specifications%29</t>
-        </is>
-      </c>
+      <c r="AZ30" t="inlineStr"/>
+      <c r="BA30" t="inlineStr"/>
+      <c r="BB30" t="inlineStr"/>
+      <c r="BC30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -9000,26 +8792,10 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="AZ31" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="BA31" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="BB31" t="inlineStr">
-        <is>
-          <t>https://www.google.com/search?q=inurl%3Ayeu.com+%28%22quick+change+connector%22+OR+%22connector%22+OR+%22quick+disconnect+connector%22+OR+%22quick+connector%22+OR+%22fluid+connector%22+OR+%22hydraulic+connector%22+or+%22hydraulic%22+or+%22fluid%22%29+%28product+OR+buy+OR+shop+OR+store+OR+price+OR+catalog+OR+%0A++++++++++++specifications%29</t>
-        </is>
-      </c>
-      <c r="BC31" t="inlineStr">
-        <is>
-          <t>https://www.google.com/search?q=inurl%3Ayeu.com+%28%22quick+change+connector%22+OR+%22connector%22+OR+%22quick+disconnect+connector%22+OR+%22quick+connector%22+OR+%22fluid+connector%22+OR+%22hydraulic+connector%22+or+%22hydraulic%22+or+%22fluid%22%29+%28product+OR+buy+OR+shop+OR+store+OR+price+OR+catalog+OR+%0A++++++++++++specifications%29</t>
-        </is>
-      </c>
+      <c r="AZ31" t="inlineStr"/>
+      <c r="BA31" t="inlineStr"/>
+      <c r="BB31" t="inlineStr"/>
+      <c r="BC31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -9277,26 +9053,10 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="AZ32" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="BA32" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="BB32" t="inlineStr">
-        <is>
-          <t>https://www.google.com/search?q=inurl%3Aairhydropower.com+%28%22quick+change+connector%22+OR+%22connector%22+OR+%22quick+disconnect+connector%22+OR+%22quick+connector%22+OR+%22fluid+connector%22+OR+%22hydraulic+connector%22+or+%22hydraulic%22+or+%22fluid%22%29+%28product+OR+buy+OR+shop+OR+store+OR+price+OR+catalog+OR+%0A++++++++++++specifications%29</t>
-        </is>
-      </c>
-      <c r="BC32" t="inlineStr">
-        <is>
-          <t>https://www.google.com/search?q=inurl%3Aairhydropower.com+%28%22quick+change+connector%22+OR+%22connector%22+OR+%22quick+disconnect+connector%22+OR+%22quick+connector%22+OR+%22fluid+connector%22+OR+%22hydraulic+connector%22+or+%22hydraulic%22+or+%22fluid%22%29+%28product+OR+buy+OR+shop+OR+store+OR+price+OR+catalog+OR+%0A++++++++++++specifications%29</t>
-        </is>
-      </c>
+      <c r="AZ32" t="inlineStr"/>
+      <c r="BA32" t="inlineStr"/>
+      <c r="BB32" t="inlineStr"/>
+      <c r="BC32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -9554,26 +9314,10 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="AZ33" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="BA33" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="BB33" t="inlineStr">
-        <is>
-          <t>https://www.google.com/search?q=inurl%3Apeigenesis.com+%28%22quick+change+connector%22+OR+%22connector%22+OR+%22quick+disconnect+connector%22+OR+%22quick+connector%22+OR+%22fluid+connector%22+OR+%22hydraulic+connector%22+or+%22hydraulic%22+or+%22fluid%22%29+%28product+OR+buy+OR+shop+OR+store+OR+price+OR+catalog+OR+%0A++++++++++++specifications%29</t>
-        </is>
-      </c>
-      <c r="BC33" t="inlineStr">
-        <is>
-          <t>https://www.google.com/search?q=inurl%3Apeigenesis.com+%28%22quick+change+connector%22+OR+%22connector%22+OR+%22quick+disconnect+connector%22+OR+%22quick+connector%22+OR+%22fluid+connector%22+OR+%22hydraulic+connector%22+or+%22hydraulic%22+or+%22fluid%22%29+%28product+OR+buy+OR+shop+OR+store+OR+price+OR+catalog+OR+%0A++++++++++++specifications%29</t>
-        </is>
-      </c>
+      <c r="AZ33" t="inlineStr"/>
+      <c r="BA33" t="inlineStr"/>
+      <c r="BB33" t="inlineStr"/>
+      <c r="BC33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -9833,16 +9577,8 @@
       </c>
       <c r="AZ34" t="inlineStr"/>
       <c r="BA34" t="inlineStr"/>
-      <c r="BB34" t="inlineStr">
-        <is>
-          <t>https://www.google.com/search?q=inurl%3Aairlinehyd.com+%28%22quick+change+connector%22+OR+%22connector%22+OR+%22quick+disconnect+connector%22+OR+%22quick+connector%22+OR+%22fluid+connector%22+OR+%22hydraulic+connector%22+or+%22hydraulic%22+or+%22fluid%22%29+%28product+OR+buy+OR+shop+OR+store+OR+price+OR+catalog+OR+%0A++++++++++++specifications%29</t>
-        </is>
-      </c>
-      <c r="BC34" t="inlineStr">
-        <is>
-          <t>https://www.google.com/search?q=inurl%3Aairlinehyd.com+%28%22quick+change+connector%22+OR+%22connector%22+OR+%22quick+disconnect+connector%22+OR+%22quick+connector%22+OR+%22fluid+connector%22+OR+%22hydraulic+connector%22+or+%22hydraulic%22+or+%22fluid%22%29+%28product+OR+buy+OR+shop+OR+store+OR+price+OR+catalog+OR+%0A++++++++++++specifications%29</t>
-        </is>
-      </c>
+      <c r="BB34" t="inlineStr"/>
+      <c r="BC34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -10102,16 +9838,8 @@
       </c>
       <c r="AZ35" t="inlineStr"/>
       <c r="BA35" t="inlineStr"/>
-      <c r="BB35" t="inlineStr">
-        <is>
-          <t>https://www.google.com/search?q=inurl%3Apowermation.com+%28%22quick+change+connector%22+OR+%22connector%22+OR+%22quick+disconnect+connector%22+OR+%22quick+connector%22+OR+%22fluid+connector%22+OR+%22hydraulic+connector%22+or+%22hydraulic%22+or+%22fluid%22%29+%28product+OR+buy+OR+shop+OR+store+OR+price+OR+catalog+OR+%0A++++++++++++specifications%29</t>
-        </is>
-      </c>
-      <c r="BC35" t="inlineStr">
-        <is>
-          <t>https://www.google.com/search?q=inurl%3Apowermation.com+%28%22quick+change+connector%22+OR+%22connector%22+OR+%22quick+disconnect+connector%22+OR+%22quick+connector%22+OR+%22fluid+connector%22+OR+%22hydraulic+connector%22+or+%22hydraulic%22+or+%22fluid%22%29+%28product+OR+buy+OR+shop+OR+store+OR+price+OR+catalog+OR+%0A++++++++++++specifications%29</t>
-        </is>
-      </c>
+      <c r="BB35" t="inlineStr"/>
+      <c r="BC35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -10371,16 +10099,8 @@
       </c>
       <c r="AZ36" t="inlineStr"/>
       <c r="BA36" t="inlineStr"/>
-      <c r="BB36" t="inlineStr">
-        <is>
-          <t>https://www.google.com/search?q=inurl%3Aturtle.com+%28%22quick+change+connector%22+OR+%22connector%22+OR+%22quick+disconnect+connector%22+OR+%22quick+connector%22+OR+%22fluid+connector%22+OR+%22hydraulic+connector%22+or+%22hydraulic%22+or+%22fluid%22%29+%28product+OR+buy+OR+shop+OR+store+OR+price+OR+catalog+OR+%0A++++++++++++specifications%29</t>
-        </is>
-      </c>
-      <c r="BC36" t="inlineStr">
-        <is>
-          <t>https://www.google.com/search?q=inurl%3Aturtle.com+%28%22quick+change+connector%22+OR+%22connector%22+OR+%22quick+disconnect+connector%22+OR+%22quick+connector%22+OR+%22fluid+connector%22+OR+%22hydraulic+connector%22+or+%22hydraulic%22+or+%22fluid%22%29+%28product+OR+buy+OR+shop+OR+store+OR+price+OR+catalog+OR+%0A++++++++++++specifications%29</t>
-        </is>
-      </c>
+      <c r="BB36" t="inlineStr"/>
+      <c r="BC36" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>